<commit_message>
merged all the different rob dataframes by riccardo
</commit_message>
<xml_diff>
--- a/02_data/rawdata/Rob_Assesment_Riccardo_Johanna21.09.2023.xlsx
+++ b/02_data/rawdata/Rob_Assesment_Riccardo_Johanna21.09.2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\Documents\PhD\UmbrellaMA\02_data\rawdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5966EF-8325-4761-9CB7-561B3ABA3A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239958B6-0AB0-4BE4-B1B4-6ADCB01EF958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Healthy_Symptoms" sheetId="1" r:id="rId1"/>
@@ -1852,7 +1852,7 @@
   <dimension ref="A1:Y13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2370,7 +2370,7 @@
   <dimension ref="A1:AK18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3049,7 +3049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31CFAEC-CE29-4C66-AC86-42076EF96F73}">
   <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="Q1" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -4042,7 +4042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2188E158-2F7E-476A-88DD-EAD34503B8C4}">
   <dimension ref="A1:AK18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>

</xml_diff>